<commit_message>
SJT + demo data
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/data_empschul_labor_lehrperson.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/data_empschul_labor_lehrperson.xlsx
@@ -8,22 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\R script\demographic data\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_ABB3F5451BDC24510042E4A75CB618A96AE60A0A" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4030D29D-718F-45C7-91BD-C4BD648C6066}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{AAA4C274-D76F-44FB-B3D7-FDB7AE4B39EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{889617BB-FFE0-440E-8568-64F6717F8280}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8196" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="empschul_labor_lehrperson" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">empschul_labor_lehrperson!$A$1:$BJ$27</definedName>
-  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="111">
   <si>
     <t>CASE</t>
   </si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>11</t>
+  </si>
+  <si>
+    <t>GTA-Kursleiterin an mehreren Schulen für Kunst, Theater, Fördern (2,5 Jahre)</t>
   </si>
 </sst>
 </file>
@@ -711,22 +711,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
-  <dimension ref="A1:BJ27"/>
+  <dimension ref="A1:BJ29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AK3" sqref="AK3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="36" width="8" customWidth="1"/>
-    <col min="37" max="37" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="37" width="8" customWidth="1"/>
     <col min="38" max="40" width="32" customWidth="1"/>
     <col min="41" max="41" width="8" customWidth="1"/>
     <col min="42" max="42" width="32" customWidth="1"/>
@@ -740,7 +738,7 @@
     <col min="63" max="1024" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -928,7 +926,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>98</v>
       </c>
@@ -1102,13 +1100,13 @@
         <v>1</v>
       </c>
       <c r="BI2" s="4">
-        <v>1.27</v>
+        <v>1.32</v>
       </c>
       <c r="BJ2" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -1282,13 +1280,13 @@
         <v>1</v>
       </c>
       <c r="BI3" s="4">
-        <v>0.93</v>
+        <v>0.95</v>
       </c>
       <c r="BJ3" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>101</v>
       </c>
@@ -1462,13 +1460,13 @@
         <v>1</v>
       </c>
       <c r="BI4" s="4">
-        <v>1.25</v>
+        <v>1.29</v>
       </c>
       <c r="BJ4" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>102</v>
       </c>
@@ -1642,13 +1640,13 @@
         <v>1</v>
       </c>
       <c r="BI5" s="4">
-        <v>1.04</v>
+        <v>1.07</v>
       </c>
       <c r="BJ5" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>104</v>
       </c>
@@ -1812,13 +1810,13 @@
         <v>1</v>
       </c>
       <c r="BI6" s="4">
-        <v>1.37</v>
+        <v>1.45</v>
       </c>
       <c r="BJ6" s="1">
-        <v>20</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="7" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>106</v>
       </c>
@@ -1992,13 +1990,13 @@
         <v>1</v>
       </c>
       <c r="BI7" s="4">
-        <v>1.61</v>
+        <v>1.64</v>
       </c>
       <c r="BJ7" s="1">
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>107</v>
       </c>
@@ -2172,13 +2170,13 @@
         <v>1</v>
       </c>
       <c r="BI8" s="4">
-        <v>1.42</v>
+        <v>1.45</v>
       </c>
       <c r="BJ8" s="1">
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>109</v>
       </c>
@@ -2344,13 +2342,13 @@
         <v>0</v>
       </c>
       <c r="BI9" s="4">
-        <v>1.45</v>
+        <v>1.5</v>
       </c>
       <c r="BJ9" s="1">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>110</v>
       </c>
@@ -2516,13 +2514,13 @@
         <v>0</v>
       </c>
       <c r="BI10" s="4">
-        <v>1.45</v>
+        <v>1.55</v>
       </c>
       <c r="BJ10" s="1">
-        <v>28</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>111</v>
       </c>
@@ -2696,13 +2694,13 @@
         <v>1</v>
       </c>
       <c r="BI11" s="4">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="BJ11" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>112</v>
       </c>
@@ -2876,13 +2874,13 @@
         <v>1</v>
       </c>
       <c r="BI12" s="4">
-        <v>1.2</v>
+        <v>1.22</v>
       </c>
       <c r="BJ12" s="1">
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>113</v>
       </c>
@@ -3058,13 +3056,13 @@
         <v>0</v>
       </c>
       <c r="BI13" s="4">
-        <v>0.84</v>
+        <v>0.86</v>
       </c>
       <c r="BJ13" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>114</v>
       </c>
@@ -3238,13 +3236,13 @@
         <v>1</v>
       </c>
       <c r="BI14" s="4">
-        <v>1.3</v>
+        <v>1.34</v>
       </c>
       <c r="BJ14" s="1">
-        <v>15</v>
+        <v>18</v>
       </c>
     </row>
-    <row r="15" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>116</v>
       </c>
@@ -3410,13 +3408,13 @@
         <v>0</v>
       </c>
       <c r="BI15" s="4">
-        <v>1.18</v>
+        <v>1.23</v>
       </c>
       <c r="BJ15" s="1">
-        <v>12</v>
+        <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>118</v>
       </c>
@@ -3590,13 +3588,13 @@
         <v>1</v>
       </c>
       <c r="BI16" s="4">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="BJ16" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>120</v>
       </c>
@@ -3765,10 +3763,10 @@
         <v>1.22</v>
       </c>
       <c r="BJ17" s="1">
-        <v>44</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="18" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>121</v>
       </c>
@@ -3919,7 +3917,7 @@
         <v>153</v>
       </c>
       <c r="AZ18" s="1">
-        <v>274</v>
+        <v>1814</v>
       </c>
       <c r="BA18" s="3"/>
       <c r="BB18" s="3">
@@ -3944,13 +3942,13 @@
         <v>0</v>
       </c>
       <c r="BI18" s="4">
-        <v>0.86</v>
+        <v>0.91</v>
       </c>
       <c r="BJ18" s="1">
-        <v>9</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>122</v>
       </c>
@@ -4119,10 +4117,10 @@
         <v>1.7</v>
       </c>
       <c r="BJ19" s="1">
-        <v>88</v>
+        <v>99</v>
       </c>
     </row>
-    <row r="20" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>123</v>
       </c>
@@ -4296,13 +4294,13 @@
         <v>1</v>
       </c>
       <c r="BI20" s="4">
-        <v>0.95</v>
+        <v>0.99</v>
       </c>
       <c r="BJ20" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="21" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>143</v>
       </c>
@@ -4476,13 +4474,13 @@
         <v>1</v>
       </c>
       <c r="BI21" s="4">
-        <v>0.76</v>
+        <v>0.78</v>
       </c>
       <c r="BJ21" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:62" ht="13.2" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>144</v>
       </c>
@@ -4649,10 +4647,10 @@
         <v>1.32</v>
       </c>
       <c r="BJ22" s="1">
-        <v>62</v>
+        <v>71</v>
       </c>
     </row>
-    <row r="23" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>145</v>
       </c>
@@ -4826,13 +4824,13 @@
         <v>0</v>
       </c>
       <c r="BI23" s="4">
-        <v>0.65</v>
+        <v>0.67</v>
       </c>
       <c r="BJ23" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>146</v>
       </c>
@@ -5006,13 +5004,13 @@
         <v>1</v>
       </c>
       <c r="BI24" s="4">
-        <v>0.63</v>
+        <v>0.66</v>
       </c>
       <c r="BJ24" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>147</v>
       </c>
@@ -5188,13 +5186,13 @@
         <v>0</v>
       </c>
       <c r="BI25" s="4">
-        <v>0.81</v>
+        <v>0.83</v>
       </c>
       <c r="BJ25" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="26" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>148</v>
       </c>
@@ -5368,13 +5366,13 @@
         <v>1</v>
       </c>
       <c r="BI26" s="4">
-        <v>1.2</v>
+        <v>1.25</v>
       </c>
       <c r="BJ26" s="1">
-        <v>10</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:62" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>149</v>
       </c>
@@ -5546,37 +5544,373 @@
         <v>1</v>
       </c>
       <c r="BI27" s="4">
-        <v>0.9</v>
+        <v>0.93</v>
       </c>
       <c r="BJ27" s="1">
         <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>150</v>
+      </c>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F28" s="3">
+        <v>44620.585578703998</v>
+      </c>
+      <c r="G28" s="1">
+        <v>4</v>
+      </c>
+      <c r="H28" s="1">
+        <v>4</v>
+      </c>
+      <c r="I28" s="1">
+        <v>4</v>
+      </c>
+      <c r="J28" s="1">
+        <v>3</v>
+      </c>
+      <c r="K28" s="1">
+        <v>3</v>
+      </c>
+      <c r="L28" s="1">
+        <v>2</v>
+      </c>
+      <c r="M28" s="1">
+        <v>4</v>
+      </c>
+      <c r="N28" s="1">
+        <v>3</v>
+      </c>
+      <c r="O28" s="1">
+        <v>4</v>
+      </c>
+      <c r="P28" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q28" s="1">
+        <v>4</v>
+      </c>
+      <c r="R28" s="1">
+        <v>2</v>
+      </c>
+      <c r="S28" s="1">
+        <v>3</v>
+      </c>
+      <c r="T28" s="1">
+        <v>3</v>
+      </c>
+      <c r="U28" s="1">
+        <v>4</v>
+      </c>
+      <c r="V28" s="1">
+        <v>3</v>
+      </c>
+      <c r="W28" s="1">
+        <v>3</v>
+      </c>
+      <c r="X28" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y28" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AA28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB28" s="1">
+        <v>4</v>
+      </c>
+      <c r="AC28" s="1">
+        <v>70</v>
+      </c>
+      <c r="AD28" s="1">
+        <v>3</v>
+      </c>
+      <c r="AE28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF28" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ28" s="1">
+        <v>24</v>
+      </c>
+      <c r="AK28" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM28" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN28" s="2"/>
+      <c r="AO28" s="1">
+        <v>120</v>
+      </c>
+      <c r="AP28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AQ28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR28" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AS28" s="1">
+        <v>40</v>
+      </c>
+      <c r="AT28" s="1">
+        <v>12</v>
+      </c>
+      <c r="AU28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV28" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AW28" s="1">
+        <v>3310</v>
+      </c>
+      <c r="AX28" s="1">
+        <v>111</v>
+      </c>
+      <c r="AY28" s="1">
+        <v>162</v>
+      </c>
+      <c r="AZ28" s="1">
+        <v>337</v>
+      </c>
+      <c r="BA28" s="3"/>
+      <c r="BB28" s="3">
+        <v>44620.627048611001</v>
+      </c>
+      <c r="BC28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD28" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE28" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF28" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG28" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI28" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="BJ28" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:62" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>151</v>
+      </c>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F29" s="3">
+        <v>44622.452106481003</v>
+      </c>
+      <c r="G29" s="1">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1">
+        <v>4</v>
+      </c>
+      <c r="J29" s="1">
+        <v>4</v>
+      </c>
+      <c r="K29" s="1">
+        <v>3</v>
+      </c>
+      <c r="L29" s="1">
+        <v>2</v>
+      </c>
+      <c r="M29" s="1">
+        <v>4</v>
+      </c>
+      <c r="N29" s="1">
+        <v>3</v>
+      </c>
+      <c r="O29" s="1">
+        <v>4</v>
+      </c>
+      <c r="P29" s="1">
+        <v>4</v>
+      </c>
+      <c r="Q29" s="1">
+        <v>4</v>
+      </c>
+      <c r="R29" s="1">
+        <v>4</v>
+      </c>
+      <c r="S29" s="1">
+        <v>4</v>
+      </c>
+      <c r="T29" s="1">
+        <v>4</v>
+      </c>
+      <c r="U29" s="1">
+        <v>4</v>
+      </c>
+      <c r="V29" s="1">
+        <v>4</v>
+      </c>
+      <c r="W29" s="1">
+        <v>4</v>
+      </c>
+      <c r="X29" s="1">
+        <v>4</v>
+      </c>
+      <c r="Y29" s="1">
+        <v>3</v>
+      </c>
+      <c r="Z29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AA29" s="1">
+        <v>4</v>
+      </c>
+      <c r="AB29" s="1">
+        <v>3</v>
+      </c>
+      <c r="AC29" s="1">
+        <v>30</v>
+      </c>
+      <c r="AD29" s="1">
+        <v>5</v>
+      </c>
+      <c r="AE29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AF29" s="1">
+        <v>2</v>
+      </c>
+      <c r="AG29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AH29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AI29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AJ29" s="1">
+        <v>23</v>
+      </c>
+      <c r="AK29" s="1">
+        <v>0</v>
+      </c>
+      <c r="AL29" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AM29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AN29" s="2"/>
+      <c r="AO29" s="1">
+        <v>121</v>
+      </c>
+      <c r="AP29" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AQ29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AR29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AS29" s="1">
+        <v>70</v>
+      </c>
+      <c r="AT29" s="1">
+        <v>16</v>
+      </c>
+      <c r="AU29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AV29" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AW29" s="1">
+        <v>56</v>
+      </c>
+      <c r="AX29" s="1">
+        <v>222</v>
+      </c>
+      <c r="AY29" s="1">
+        <v>205</v>
+      </c>
+      <c r="AZ29" s="1">
+        <v>483</v>
+      </c>
+      <c r="BA29" s="3"/>
+      <c r="BB29" s="3">
+        <v>44622.457708333</v>
+      </c>
+      <c r="BC29" s="1">
+        <v>1</v>
+      </c>
+      <c r="BD29" s="1">
+        <v>0</v>
+      </c>
+      <c r="BE29" s="1">
+        <v>3</v>
+      </c>
+      <c r="BF29" s="1">
+        <v>3</v>
+      </c>
+      <c r="BG29" s="1">
+        <v>3</v>
+      </c>
+      <c r="BH29" s="1">
+        <v>1</v>
+      </c>
+      <c r="BI29" s="4">
+        <v>0.8</v>
+      </c>
+      <c r="BJ29" s="1">
+        <v>2</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:BJ27" xr:uid="{3FC51B6A-8599-4FE6-A419-9B903E42ED08}">
-    <filterColumn colId="40">
-      <filters>
-        <filter val="101"/>
-        <filter val="102"/>
-        <filter val="103"/>
-        <filter val="104"/>
-        <filter val="105"/>
-        <filter val="106"/>
-        <filter val="107"/>
-        <filter val="108"/>
-        <filter val="109"/>
-        <filter val="110"/>
-        <filter val="112"/>
-        <filter val="113"/>
-        <filter val="114"/>
-        <filter val="115"/>
-        <filter val="116"/>
-        <filter val="117"/>
-        <filter val="118"/>
-        <filter val="119"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.5" right="0.5" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
   <headerFooter>

</xml_diff>

<commit_message>
method paper demo data
</commit_message>
<xml_diff>
--- a/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/data_empschul_labor_lehrperson.xlsx
+++ b/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/data_empschul_labor_lehrperson.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20383"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mk99feta\OneDrive\Dokumente\GitHub\Mandy-PhD\01_studies\01_Laborstudie ProVisioNET\R script\demographic data\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/505858402c07da9d/Dokumente/GitHub/Mandy-PhD/01_studies/01_Laborstudie ProVisioNET/R script/demographic data/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{AAA4C274-D76F-44FB-B3D7-FDB7AE4B39EC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{889617BB-FFE0-440E-8568-64F6717F8280}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3FD3AF59-6B7F-438F-BDD2-26A65CBEF76D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" tabRatio="212" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="121">
   <si>
     <t>CASE</t>
   </si>
@@ -148,6 +148,9 @@
     <t>LI10_05</t>
   </si>
   <si>
+    <t>LI16_05</t>
+  </si>
+  <si>
     <t>LI07</t>
   </si>
   <si>
@@ -166,6 +169,15 @@
     <t>LI14_01</t>
   </si>
   <si>
+    <t>LI17</t>
+  </si>
+  <si>
+    <t>LI17_01</t>
+  </si>
+  <si>
+    <t>LI18</t>
+  </si>
+  <si>
     <t>TIME001</t>
   </si>
   <si>
@@ -220,6 +232,9 @@
     <t>Spanisch</t>
   </si>
   <si>
+    <t>7</t>
+  </si>
+  <si>
     <t>3</t>
   </si>
   <si>
@@ -229,6 +244,9 @@
     <t>Geschichte</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>10</t>
   </si>
   <si>
@@ -241,6 +259,9 @@
     <t>Deutsch</t>
   </si>
   <si>
+    <t>11</t>
+  </si>
+  <si>
     <t>8</t>
   </si>
   <si>
@@ -250,6 +271,9 @@
     <t>Ethik</t>
   </si>
   <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>FSJ Politik und jugendpolitische Bildungsarbeit (Klasse 5-10)</t>
   </si>
   <si>
@@ -262,15 +286,15 @@
     <t>ev. Religion</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>AG an Schulen, Trainertätigkeit, Nachhilfe(einzel)</t>
   </si>
   <si>
     <t>Gewi</t>
   </si>
   <si>
+    <t>Hauptausbildungsleiterin am Seminar für das höhere Lehramt an Gymnasien</t>
+  </si>
+  <si>
     <t>Mathematik</t>
   </si>
   <si>
@@ -307,6 +331,9 @@
     <t>NaWi-Profil</t>
   </si>
   <si>
+    <t>Fachberater für Begabungsförderung</t>
+  </si>
+  <si>
     <t>3.</t>
   </si>
   <si>
@@ -316,7 +343,13 @@
     <t>TC</t>
   </si>
   <si>
-    <t>5</t>
+    <t>Dozentin an Universität Leipzig</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Hauptausbildungsleiterin für zweiten Bildungsabschnitt an Lehrer:innenausbildungsstätte Leipzig</t>
   </si>
   <si>
     <t>Biologie</t>
@@ -328,6 +361,9 @@
     <t>Kunst</t>
   </si>
   <si>
+    <t>Dozent an Universität Leipzig</t>
+  </si>
+  <si>
     <t>Geistige Entwicklung</t>
   </si>
   <si>
@@ -337,9 +373,6 @@
     <t>Informatik</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Trainer Callcenter</t>
   </si>
   <si>
@@ -347,9 +380,6 @@
   </si>
   <si>
     <t>Nachhilfe, Hausaufgabenbetreuung, FSJ an einer Schule</t>
-  </si>
-  <si>
-    <t>11</t>
   </si>
   <si>
     <t>GTA-Kursleiterin an mehreren Schulen für Kunst, Theater, Fördern (2,5 Jahre)</t>
@@ -711,34 +741,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BJ29"/>
+  <dimension ref="A1:BN29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AK1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AK3" sqref="AK3"/>
+      <selection pane="bottomLeft" activeCell="X3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8" customWidth="1"/>
     <col min="2" max="4" width="20" customWidth="1"/>
     <col min="5" max="5" width="16" customWidth="1"/>
     <col min="6" max="6" width="20" customWidth="1"/>
-    <col min="7" max="37" width="8" customWidth="1"/>
+    <col min="7" max="35" width="8" customWidth="1"/>
+    <col min="36" max="36" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="8" customWidth="1"/>
     <col min="38" max="40" width="32" customWidth="1"/>
     <col min="41" max="41" width="8" customWidth="1"/>
-    <col min="42" max="42" width="32" customWidth="1"/>
-    <col min="43" max="43" width="8" customWidth="1"/>
-    <col min="44" max="44" width="32" customWidth="1"/>
-    <col min="45" max="47" width="8" customWidth="1"/>
-    <col min="48" max="48" width="32" customWidth="1"/>
-    <col min="49" max="52" width="5" customWidth="1"/>
-    <col min="53" max="54" width="20" customWidth="1"/>
-    <col min="55" max="62" width="8" customWidth="1"/>
-    <col min="63" max="1024" width="11.44140625"/>
+    <col min="42" max="43" width="32" customWidth="1"/>
+    <col min="44" max="44" width="8" customWidth="1"/>
+    <col min="45" max="45" width="32" customWidth="1"/>
+    <col min="46" max="48" width="8" customWidth="1"/>
+    <col min="49" max="49" width="32" customWidth="1"/>
+    <col min="50" max="50" width="8" customWidth="1"/>
+    <col min="51" max="51" width="32" customWidth="1"/>
+    <col min="52" max="52" width="8" customWidth="1"/>
+    <col min="53" max="56" width="5" customWidth="1"/>
+    <col min="57" max="58" width="20" customWidth="1"/>
+    <col min="59" max="66" width="8" customWidth="1"/>
+    <col min="67" max="1024" width="11.44140625"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -925,18 +960,30 @@
       <c r="BJ1" s="5" t="s">
         <v>61</v>
       </c>
+      <c r="BK1" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>63</v>
+      </c>
+      <c r="BM1" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="BN1" s="5" t="s">
+        <v>65</v>
+      </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>98</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F2" s="3">
         <v>44398.681701389003</v>
@@ -1035,88 +1082,96 @@
         <v>0</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AN2" s="2"/>
       <c r="AO2" s="1">
         <v>101</v>
       </c>
       <c r="AP2" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AQ2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR2" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS2" s="1">
+        <v>69</v>
+      </c>
+      <c r="AQ2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AT2" s="1">
         <v>5</v>
       </c>
-      <c r="AT2" s="1">
-        <v>4</v>
-      </c>
       <c r="AU2" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV2" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="AW2" s="1">
-        <v>42</v>
-      </c>
-      <c r="AX2" s="1">
-        <v>54</v>
-      </c>
-      <c r="AY2" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV2" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="AX2" s="1"/>
+      <c r="AY2" s="2"/>
+      <c r="AZ2" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA2" s="1">
+        <v>120</v>
+      </c>
+      <c r="BB2" s="1">
+        <v>93</v>
+      </c>
+      <c r="BC2" s="1">
         <v>215</v>
       </c>
-      <c r="AZ2" s="1">
-        <v>311</v>
-      </c>
-      <c r="BA2" s="3"/>
-      <c r="BB2" s="3">
-        <v>44398.685300926001</v>
-      </c>
-      <c r="BC2" s="1">
-        <v>1</v>
-      </c>
       <c r="BD2" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE2" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF2" s="1">
-        <v>3</v>
+        <v>428</v>
+      </c>
+      <c r="BE2" s="3"/>
+      <c r="BF2" s="3">
+        <v>44645.921053241</v>
       </c>
       <c r="BG2" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH2" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI2" s="4">
-        <v>1.32</v>
+        <v>0</v>
+      </c>
+      <c r="BI2" s="1">
+        <v>2</v>
       </c>
       <c r="BJ2" s="1">
-        <v>19</v>
+        <v>3</v>
+      </c>
+      <c r="BK2" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL2" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM2" s="4">
+        <v>0.92</v>
+      </c>
+      <c r="BN2" s="1">
+        <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F3" s="3">
         <v>44404.681817129996</v>
@@ -1215,88 +1270,96 @@
         <v>0</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AM3" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AN3" s="2"/>
       <c r="AO3" s="1">
         <v>102</v>
       </c>
       <c r="AP3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR3" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS3" s="1">
+        <v>73</v>
+      </c>
+      <c r="AQ3" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS3" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AT3" s="1">
         <v>23</v>
       </c>
-      <c r="AT3" s="1">
+      <c r="AU3" s="1">
         <v>36</v>
       </c>
-      <c r="AU3" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="AW3" s="1">
-        <v>72</v>
-      </c>
-      <c r="AX3" s="1">
-        <v>113</v>
-      </c>
-      <c r="AY3" s="1">
+      <c r="AV3" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW3" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="AX3" s="1"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA3" s="1">
+        <v>95</v>
+      </c>
+      <c r="BB3" s="1">
+        <v>132</v>
+      </c>
+      <c r="BC3" s="1">
         <v>147</v>
       </c>
-      <c r="AZ3" s="1">
-        <v>332</v>
-      </c>
-      <c r="BA3" s="3"/>
-      <c r="BB3" s="3">
-        <v>44404.685659722003</v>
-      </c>
-      <c r="BC3" s="1">
-        <v>1</v>
-      </c>
       <c r="BD3" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE3" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF3" s="1">
-        <v>3</v>
+        <v>374</v>
+      </c>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3">
+        <v>44645.922812500001</v>
       </c>
       <c r="BG3" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH3" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI3" s="4">
-        <v>0.95</v>
+        <v>0</v>
+      </c>
+      <c r="BI3" s="1">
+        <v>2</v>
       </c>
       <c r="BJ3" s="1">
         <v>3</v>
       </c>
+      <c r="BK3" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL3" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM3" s="4">
+        <v>1</v>
+      </c>
+      <c r="BN3" s="1">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>101</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F4" s="3">
         <v>44405.615405092998</v>
@@ -1395,88 +1458,98 @@
         <v>0</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AN4" s="2"/>
       <c r="AO4" s="1">
         <v>103</v>
       </c>
       <c r="AP4" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR4" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS4" s="1">
+        <v>78</v>
+      </c>
+      <c r="AQ4" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AR4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT4" s="1">
         <v>28</v>
       </c>
-      <c r="AT4" s="1">
+      <c r="AU4" s="1">
         <v>8</v>
       </c>
-      <c r="AU4" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV4" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW4" s="1">
-        <v>43</v>
+      <c r="AV4" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW4" s="2" t="s">
+        <v>81</v>
       </c>
       <c r="AX4" s="1">
-        <v>63</v>
-      </c>
-      <c r="AY4" s="1">
+        <v>-9</v>
+      </c>
+      <c r="AY4" s="2"/>
+      <c r="AZ4" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA4" s="1">
+        <v>366</v>
+      </c>
+      <c r="BB4" s="1">
+        <v>347</v>
+      </c>
+      <c r="BC4" s="1">
         <v>176</v>
       </c>
-      <c r="AZ4" s="1">
-        <v>282</v>
-      </c>
-      <c r="BA4" s="3"/>
-      <c r="BB4" s="3">
-        <v>44405.618680555999</v>
-      </c>
-      <c r="BC4" s="1">
-        <v>1</v>
-      </c>
       <c r="BD4" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE4" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF4" s="1">
-        <v>3</v>
+        <v>646</v>
+      </c>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3">
+        <v>44645.923449073998</v>
       </c>
       <c r="BG4" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH4" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI4" s="4">
-        <v>1.29</v>
+        <v>0</v>
+      </c>
+      <c r="BI4" s="1">
+        <v>2</v>
       </c>
       <c r="BJ4" s="1">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="BK4" s="1">
+        <v>5</v>
+      </c>
+      <c r="BL4" s="1">
+        <v>3</v>
+      </c>
+      <c r="BM4" s="4">
+        <v>0.53</v>
+      </c>
+      <c r="BN4" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>102</v>
       </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F5" s="3">
         <v>44413.621111111002</v>
@@ -1575,88 +1648,96 @@
         <v>0</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AN5" s="2"/>
       <c r="AO5" s="1">
         <v>104</v>
       </c>
       <c r="AP5" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="AQ5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR5" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS5" s="1">
+        <v>82</v>
+      </c>
+      <c r="AQ5" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS5" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT5" s="1">
         <v>14</v>
       </c>
-      <c r="AT5" s="1">
+      <c r="AU5" s="1">
         <v>24</v>
       </c>
-      <c r="AU5" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV5" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="AW5" s="1">
-        <v>44</v>
-      </c>
-      <c r="AX5" s="1">
-        <v>119</v>
-      </c>
-      <c r="AY5" s="1">
-        <v>173</v>
-      </c>
+      <c r="AV5" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW5" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX5" s="1"/>
+      <c r="AY5" s="2"/>
       <c r="AZ5" s="1">
-        <v>336</v>
-      </c>
-      <c r="BA5" s="3"/>
-      <c r="BB5" s="3">
-        <v>44413.625</v>
+        <v>3</v>
+      </c>
+      <c r="BA5" s="1">
+        <v>65</v>
+      </c>
+      <c r="BB5" s="1">
+        <v>128</v>
       </c>
       <c r="BC5" s="1">
-        <v>1</v>
+        <v>439</v>
       </c>
       <c r="BD5" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE5" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF5" s="1">
-        <v>3</v>
+        <v>372</v>
+      </c>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3">
+        <v>44645.927395833001</v>
       </c>
       <c r="BG5" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="BH5" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI5" s="4">
-        <v>1.07</v>
+        <v>0</v>
+      </c>
+      <c r="BI5" s="1">
+        <v>3</v>
       </c>
       <c r="BJ5" s="1">
+        <v>3</v>
+      </c>
+      <c r="BK5" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL5" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM5" s="4">
+        <v>0.9</v>
+      </c>
+      <c r="BN5" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>104</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F6" s="3">
         <v>44439.542256943998</v>
@@ -1755,78 +1836,88 @@
         <v>29</v>
       </c>
       <c r="AL6" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AN6" s="2"/>
       <c r="AO6" s="1">
         <v>201</v>
       </c>
       <c r="AP6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ6" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR6" s="2"/>
-      <c r="AS6" s="1"/>
+        <v>77</v>
+      </c>
+      <c r="AQ6" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS6" s="2"/>
       <c r="AT6" s="1"/>
       <c r="AU6" s="1"/>
-      <c r="AV6" s="2"/>
-      <c r="AW6" s="1">
-        <v>57</v>
-      </c>
+      <c r="AV6" s="1"/>
+      <c r="AW6" s="2"/>
       <c r="AX6" s="1">
-        <v>38</v>
-      </c>
-      <c r="AY6" s="1">
+        <v>2</v>
+      </c>
+      <c r="AY6" s="2"/>
+      <c r="AZ6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA6" s="1">
+        <v>82</v>
+      </c>
+      <c r="BB6" s="1">
+        <v>72</v>
+      </c>
+      <c r="BC6" s="1">
         <v>193</v>
       </c>
-      <c r="AZ6" s="1">
-        <v>288</v>
-      </c>
-      <c r="BA6" s="3"/>
-      <c r="BB6" s="3">
-        <v>44439.545590278001</v>
-      </c>
-      <c r="BC6" s="1">
-        <v>1</v>
-      </c>
       <c r="BD6" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE6" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF6" s="1">
-        <v>3</v>
+        <v>347</v>
+      </c>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3">
+        <v>44645.925219907003</v>
       </c>
       <c r="BG6" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH6" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI6" s="4">
-        <v>1.45</v>
+        <v>0</v>
+      </c>
+      <c r="BI6" s="1">
+        <v>2</v>
       </c>
       <c r="BJ6" s="1">
-        <v>24</v>
+        <v>3</v>
+      </c>
+      <c r="BK6" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL6" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM6" s="4">
+        <v>1.18</v>
+      </c>
+      <c r="BN6" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>106</v>
       </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F7" s="3">
         <v>44440.664108796002</v>
@@ -1925,88 +2016,96 @@
         <v>0</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AM7" s="2" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
       <c r="AN7" s="2"/>
       <c r="AO7" s="1">
         <v>105</v>
       </c>
       <c r="AP7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AQ7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AS7" s="1">
+        <v>85</v>
+      </c>
+      <c r="AQ7" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS7" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AT7" s="1">
         <v>25</v>
       </c>
-      <c r="AT7" s="1">
+      <c r="AU7" s="1">
         <v>10</v>
       </c>
-      <c r="AU7" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV7" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="AW7" s="1">
-        <v>22</v>
-      </c>
-      <c r="AX7" s="1">
-        <v>93</v>
-      </c>
-      <c r="AY7" s="1">
+      <c r="AV7" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW7" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AX7" s="1"/>
+      <c r="AY7" s="2"/>
+      <c r="AZ7" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA7" s="1">
+        <v>48</v>
+      </c>
+      <c r="BB7" s="1">
+        <v>104</v>
+      </c>
+      <c r="BC7" s="1">
         <v>161</v>
       </c>
-      <c r="AZ7" s="1">
-        <v>276</v>
-      </c>
-      <c r="BA7" s="3"/>
-      <c r="BB7" s="3">
-        <v>44440.667303241004</v>
-      </c>
-      <c r="BC7" s="1">
-        <v>1</v>
-      </c>
       <c r="BD7" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE7" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF7" s="1">
-        <v>3</v>
+        <v>313</v>
+      </c>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3">
+        <v>44645.928645833003</v>
       </c>
       <c r="BG7" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH7" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI7" s="4">
-        <v>1.64</v>
+        <v>0</v>
+      </c>
+      <c r="BI7" s="1">
+        <v>2</v>
       </c>
       <c r="BJ7" s="1">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="BK7" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL7" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM7" s="4">
+        <v>1.37</v>
+      </c>
+      <c r="BN7" s="1">
+        <v>18</v>
       </c>
     </row>
-    <row r="8" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>107</v>
       </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F8" s="3">
         <v>44454.462800925998</v>
@@ -2105,88 +2204,96 @@
         <v>0</v>
       </c>
       <c r="AL8" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AM8" s="2" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="AN8" s="2"/>
       <c r="AO8" s="1">
         <v>106</v>
       </c>
       <c r="AP8" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="AQ8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR8" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="AS8" s="1">
+        <v>87</v>
+      </c>
+      <c r="AQ8" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS8" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AT8" s="1">
         <v>20</v>
       </c>
-      <c r="AT8" s="1">
-        <v>4</v>
-      </c>
       <c r="AU8" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV8" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="AW8" s="1">
-        <v>41</v>
-      </c>
-      <c r="AX8" s="1">
-        <v>93</v>
-      </c>
-      <c r="AY8" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV8" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW8" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AX8" s="1"/>
+      <c r="AY8" s="2"/>
+      <c r="AZ8" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA8" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB8" s="1">
+        <v>104</v>
+      </c>
+      <c r="BC8" s="1">
         <v>94</v>
       </c>
-      <c r="AZ8" s="1">
-        <v>228</v>
-      </c>
-      <c r="BA8" s="3"/>
-      <c r="BB8" s="3">
-        <v>44454.465439815001</v>
-      </c>
-      <c r="BC8" s="1">
-        <v>1</v>
-      </c>
       <c r="BD8" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE8" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF8" s="1">
-        <v>3</v>
+        <v>253</v>
+      </c>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3">
+        <v>44645.929155092999</v>
       </c>
       <c r="BG8" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH8" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI8" s="4">
-        <v>1.45</v>
+        <v>0</v>
+      </c>
+      <c r="BI8" s="1">
+        <v>2</v>
       </c>
       <c r="BJ8" s="1">
-        <v>23</v>
+        <v>3</v>
+      </c>
+      <c r="BK8" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL8" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM8" s="4">
+        <v>1.55</v>
+      </c>
+      <c r="BN8" s="1">
+        <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>109</v>
       </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F9" s="3">
         <v>44466.706238425999</v>
@@ -2285,55 +2392,55 @@
         <v>32</v>
       </c>
       <c r="AL9" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AM9" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AN9" s="2" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="AO9" s="1">
         <v>202</v>
       </c>
       <c r="AP9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ9" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="1"/>
+        <v>73</v>
+      </c>
+      <c r="AQ9" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR9" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS9" s="2"/>
       <c r="AT9" s="1"/>
       <c r="AU9" s="1"/>
-      <c r="AV9" s="2"/>
-      <c r="AW9" s="1">
-        <v>66</v>
-      </c>
+      <c r="AV9" s="1"/>
+      <c r="AW9" s="2"/>
       <c r="AX9" s="1">
-        <v>28</v>
-      </c>
-      <c r="AY9" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY9" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AZ9" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA9" s="1">
+        <v>96</v>
+      </c>
+      <c r="BB9" s="1">
+        <v>58</v>
+      </c>
+      <c r="BC9" s="1">
         <v>330</v>
       </c>
-      <c r="AZ9" s="1">
-        <v>269</v>
-      </c>
-      <c r="BA9" s="3"/>
-      <c r="BB9" s="3">
-        <v>44466.711145832996</v>
-      </c>
-      <c r="BC9" s="1">
-        <v>1</v>
-      </c>
       <c r="BD9" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE9" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF9" s="1">
-        <v>3</v>
+        <v>333</v>
+      </c>
+      <c r="BE9" s="3"/>
+      <c r="BF9" s="3">
+        <v>44645.930092593</v>
       </c>
       <c r="BG9" s="1">
         <v>0</v>
@@ -2341,24 +2448,36 @@
       <c r="BH9" s="1">
         <v>0</v>
       </c>
-      <c r="BI9" s="4">
-        <v>1.5</v>
+      <c r="BI9" s="1">
+        <v>2</v>
       </c>
       <c r="BJ9" s="1">
-        <v>36</v>
+        <v>3</v>
+      </c>
+      <c r="BK9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL9" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM9" s="4">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="BN9" s="1">
+        <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>110</v>
       </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F10" s="3">
         <v>44474.657476852</v>
@@ -2457,55 +2576,53 @@
         <v>3</v>
       </c>
       <c r="AL10" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AN10" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="AO10" s="1">
         <v>203</v>
       </c>
       <c r="AP10" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ10" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="AQ10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS10" s="2"/>
       <c r="AT10" s="1"/>
       <c r="AU10" s="1"/>
-      <c r="AV10" s="2"/>
-      <c r="AW10" s="1">
-        <v>64</v>
-      </c>
+      <c r="AV10" s="1"/>
+      <c r="AW10" s="2"/>
       <c r="AX10" s="1">
-        <v>30</v>
-      </c>
-      <c r="AY10" s="1">
+        <v>2</v>
+      </c>
+      <c r="AY10" s="2"/>
+      <c r="AZ10" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA10" s="1">
+        <v>85</v>
+      </c>
+      <c r="BB10" s="1">
+        <v>55</v>
+      </c>
+      <c r="BC10" s="1">
         <v>256</v>
       </c>
-      <c r="AZ10" s="1">
-        <v>350</v>
-      </c>
-      <c r="BA10" s="3"/>
-      <c r="BB10" s="3">
-        <v>44474.661527778</v>
-      </c>
-      <c r="BC10" s="1">
-        <v>1</v>
-      </c>
       <c r="BD10" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE10" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF10" s="1">
-        <v>3</v>
+        <v>396</v>
+      </c>
+      <c r="BE10" s="3"/>
+      <c r="BF10" s="3">
+        <v>44645.930983796003</v>
       </c>
       <c r="BG10" s="1">
         <v>0</v>
@@ -2513,24 +2630,36 @@
       <c r="BH10" s="1">
         <v>0</v>
       </c>
-      <c r="BI10" s="4">
-        <v>1.55</v>
+      <c r="BI10" s="1">
+        <v>2</v>
       </c>
       <c r="BJ10" s="1">
-        <v>33</v>
+        <v>3</v>
+      </c>
+      <c r="BK10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL10" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM10" s="4">
+        <v>1.24</v>
+      </c>
+      <c r="BN10" s="1">
+        <v>17</v>
       </c>
     </row>
-    <row r="11" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>111</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F11" s="3">
         <v>44475.495243056001</v>
@@ -2629,88 +2758,96 @@
         <v>0</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AM11" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AN11" s="2"/>
       <c r="AO11" s="1">
         <v>107</v>
       </c>
       <c r="AP11" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR11" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS11" s="1">
+        <v>91</v>
+      </c>
+      <c r="AQ11" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS11" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT11" s="1">
         <v>50</v>
       </c>
-      <c r="AT11" s="1">
+      <c r="AU11" s="1">
         <v>12</v>
       </c>
-      <c r="AU11" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV11" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AW11" s="1">
-        <v>61</v>
-      </c>
-      <c r="AX11" s="1">
-        <v>177</v>
-      </c>
-      <c r="AY11" s="1">
+      <c r="AV11" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AX11" s="1"/>
+      <c r="AY11" s="2"/>
+      <c r="AZ11" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA11" s="1">
+        <v>81</v>
+      </c>
+      <c r="BB11" s="1">
+        <v>184</v>
+      </c>
+      <c r="BC11" s="1">
         <v>220</v>
       </c>
-      <c r="AZ11" s="1">
-        <v>458</v>
-      </c>
-      <c r="BA11" s="3"/>
-      <c r="BB11" s="3">
-        <v>44475.500555555998</v>
-      </c>
-      <c r="BC11" s="1">
-        <v>1</v>
-      </c>
       <c r="BD11" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE11" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF11" s="1">
-        <v>3</v>
+        <v>485</v>
+      </c>
+      <c r="BE11" s="3"/>
+      <c r="BF11" s="3">
+        <v>44645.931446759001</v>
       </c>
       <c r="BG11" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH11" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI11" s="4">
-        <v>0.78</v>
+        <v>0</v>
+      </c>
+      <c r="BI11" s="1">
+        <v>2</v>
       </c>
       <c r="BJ11" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="BK11" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL11" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM11" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="BN11" s="1">
+        <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>112</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F12" s="3">
         <v>44482.493587962999</v>
@@ -2809,88 +2946,96 @@
         <v>0</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AM12" s="2" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="AN12" s="2"/>
       <c r="AO12" s="1">
         <v>108</v>
       </c>
       <c r="AP12" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="AQ12" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR12" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS12" s="1">
+        <v>77</v>
+      </c>
+      <c r="AQ12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS12" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT12" s="1">
         <v>30</v>
       </c>
-      <c r="AT12" s="1">
+      <c r="AU12" s="1">
         <v>14</v>
       </c>
-      <c r="AU12" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW12" s="1">
-        <v>28</v>
-      </c>
-      <c r="AX12" s="1">
-        <v>132</v>
-      </c>
-      <c r="AY12" s="1">
+      <c r="AV12" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW12" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX12" s="1"/>
+      <c r="AY12" s="2"/>
+      <c r="AZ12" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA12" s="1">
+        <v>49</v>
+      </c>
+      <c r="BB12" s="1">
+        <v>138</v>
+      </c>
+      <c r="BC12" s="1">
         <v>241</v>
       </c>
-      <c r="AZ12" s="1">
-        <v>401</v>
-      </c>
-      <c r="BA12" s="3"/>
-      <c r="BB12" s="3">
-        <v>44482.498229167002</v>
-      </c>
-      <c r="BC12" s="1">
-        <v>1</v>
-      </c>
       <c r="BD12" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE12" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF12" s="1">
-        <v>3</v>
+        <v>428</v>
+      </c>
+      <c r="BE12" s="3"/>
+      <c r="BF12" s="3">
+        <v>44645.932442129997</v>
       </c>
       <c r="BG12" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH12" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI12" s="4">
-        <v>1.22</v>
+        <v>0</v>
+      </c>
+      <c r="BI12" s="1">
+        <v>2</v>
       </c>
       <c r="BJ12" s="1">
-        <v>21</v>
+        <v>3</v>
+      </c>
+      <c r="BK12" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL12" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM12" s="4">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="BN12" s="1">
+        <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>113</v>
       </c>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F13" s="3">
         <v>44487.663703703998</v>
@@ -2989,65 +3134,61 @@
         <v>0</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AM13" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="AN13" s="2" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
       <c r="AO13" s="1">
         <v>109</v>
       </c>
       <c r="AP13" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR13" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AS13" s="1">
+        <v>96</v>
+      </c>
+      <c r="AQ13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS13" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="AT13" s="1">
         <v>60</v>
       </c>
-      <c r="AT13" s="1">
+      <c r="AU13" s="1">
         <v>12</v>
       </c>
-      <c r="AU13" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV13" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW13" s="1">
-        <v>50</v>
-      </c>
-      <c r="AX13" s="1">
-        <v>143</v>
-      </c>
-      <c r="AY13" s="1">
+      <c r="AV13" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW13" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="AX13" s="1"/>
+      <c r="AY13" s="2"/>
+      <c r="AZ13" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA13" s="1">
+        <v>65</v>
+      </c>
+      <c r="BB13" s="1">
+        <v>154</v>
+      </c>
+      <c r="BC13" s="1">
         <v>252</v>
       </c>
-      <c r="AZ13" s="1">
-        <v>445</v>
-      </c>
-      <c r="BA13" s="3"/>
-      <c r="BB13" s="3">
-        <v>44487.668854167001</v>
-      </c>
-      <c r="BC13" s="1">
-        <v>1</v>
-      </c>
       <c r="BD13" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE13" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF13" s="1">
-        <v>3</v>
+        <v>471</v>
+      </c>
+      <c r="BE13" s="3"/>
+      <c r="BF13" s="3">
+        <v>44645.932939815</v>
       </c>
       <c r="BG13" s="1">
         <v>0</v>
@@ -3055,24 +3196,36 @@
       <c r="BH13" s="1">
         <v>0</v>
       </c>
-      <c r="BI13" s="4">
-        <v>0.86</v>
+      <c r="BI13" s="1">
+        <v>2</v>
       </c>
       <c r="BJ13" s="1">
-        <v>5</v>
+        <v>3</v>
+      </c>
+      <c r="BK13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL13" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM13" s="4">
+        <v>0.95</v>
+      </c>
+      <c r="BN13" s="1">
+        <v>8</v>
       </c>
     </row>
-    <row r="14" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>114</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F14" s="3">
         <v>44508.584768519002</v>
@@ -3171,88 +3324,96 @@
         <v>0</v>
       </c>
       <c r="AL14" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AM14" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AN14" s="2"/>
       <c r="AO14" s="1">
         <v>110</v>
       </c>
       <c r="AP14" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS14" s="1">
+        <v>91</v>
+      </c>
+      <c r="AQ14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS14" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT14" s="1">
         <v>30</v>
       </c>
-      <c r="AT14" s="1">
+      <c r="AU14" s="1">
         <v>12</v>
       </c>
-      <c r="AU14" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV14" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AW14" s="1">
-        <v>37</v>
-      </c>
-      <c r="AX14" s="1">
-        <v>66</v>
-      </c>
-      <c r="AY14" s="1">
+      <c r="AV14" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW14" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AX14" s="1"/>
+      <c r="AY14" s="2"/>
+      <c r="AZ14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA14" s="1">
+        <v>55</v>
+      </c>
+      <c r="BB14" s="1">
+        <v>74</v>
+      </c>
+      <c r="BC14" s="1">
         <v>182</v>
       </c>
-      <c r="AZ14" s="1">
-        <v>285</v>
-      </c>
-      <c r="BA14" s="3"/>
-      <c r="BB14" s="3">
-        <v>44508.588078704001</v>
-      </c>
-      <c r="BC14" s="1">
-        <v>1</v>
-      </c>
       <c r="BD14" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE14" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF14" s="1">
-        <v>3</v>
+        <v>311</v>
+      </c>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3">
+        <v>44645.933460647997</v>
       </c>
       <c r="BG14" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH14" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI14" s="4">
-        <v>1.34</v>
+        <v>0</v>
+      </c>
+      <c r="BI14" s="1">
+        <v>2</v>
       </c>
       <c r="BJ14" s="1">
-        <v>18</v>
+        <v>3</v>
+      </c>
+      <c r="BK14" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL14" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM14" s="4">
+        <v>1.38</v>
+      </c>
+      <c r="BN14" s="1">
+        <v>19</v>
       </c>
     </row>
-    <row r="15" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>116</v>
       </c>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F15" s="3">
         <v>44512.483414351998</v>
@@ -3351,55 +3512,55 @@
         <v>37</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AM15" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AN15" s="2" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="AO15" s="1">
         <v>204</v>
       </c>
       <c r="AP15" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ15" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR15" s="2"/>
-      <c r="AS15" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="AQ15" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR15" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS15" s="2"/>
       <c r="AT15" s="1"/>
       <c r="AU15" s="1"/>
-      <c r="AV15" s="2"/>
-      <c r="AW15" s="1">
-        <v>80</v>
-      </c>
+      <c r="AV15" s="1"/>
+      <c r="AW15" s="2"/>
       <c r="AX15" s="1">
-        <v>57</v>
-      </c>
-      <c r="AY15" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY15" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AZ15" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA15" s="1">
+        <v>110</v>
+      </c>
+      <c r="BB15" s="1">
+        <v>83</v>
+      </c>
+      <c r="BC15" s="1">
         <v>131</v>
       </c>
-      <c r="AZ15" s="1">
-        <v>268</v>
-      </c>
-      <c r="BA15" s="3"/>
-      <c r="BB15" s="3">
-        <v>44512.486516204001</v>
-      </c>
-      <c r="BC15" s="1">
-        <v>1</v>
-      </c>
       <c r="BD15" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE15" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF15" s="1">
-        <v>3</v>
+        <v>324</v>
+      </c>
+      <c r="BE15" s="3"/>
+      <c r="BF15" s="3">
+        <v>44645.934293981001</v>
       </c>
       <c r="BG15" s="1">
         <v>0</v>
@@ -3407,24 +3568,36 @@
       <c r="BH15" s="1">
         <v>0</v>
       </c>
-      <c r="BI15" s="4">
-        <v>1.23</v>
+      <c r="BI15" s="1">
+        <v>2</v>
       </c>
       <c r="BJ15" s="1">
-        <v>15</v>
+        <v>3</v>
+      </c>
+      <c r="BK15" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL15" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM15" s="4">
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="BN15" s="1">
+        <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>118</v>
       </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F16" s="3">
         <v>44515.681516204</v>
@@ -3523,88 +3696,96 @@
         <v>0</v>
       </c>
       <c r="AL16" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM16" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AN16" s="2"/>
       <c r="AO16" s="1">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="AP16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ16" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR16" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="AS16" s="1">
-        <v>2</v>
+        <v>92</v>
+      </c>
+      <c r="AQ16" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="AR16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS16" s="2" t="s">
+        <v>104</v>
       </c>
       <c r="AT16" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="AU16" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV16" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="AW16" s="1">
-        <v>72</v>
-      </c>
-      <c r="AX16" s="1">
-        <v>85</v>
-      </c>
-      <c r="AY16" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV16" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW16" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX16" s="1"/>
+      <c r="AY16" s="2"/>
+      <c r="AZ16" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA16" s="1">
+        <v>257</v>
+      </c>
+      <c r="BB16" s="1">
+        <v>93</v>
+      </c>
+      <c r="BC16" s="1">
         <v>170</v>
       </c>
-      <c r="AZ16" s="1">
-        <v>327</v>
-      </c>
-      <c r="BA16" s="3"/>
-      <c r="BB16" s="3">
-        <v>44515.685300926001</v>
-      </c>
-      <c r="BC16" s="1">
-        <v>1</v>
-      </c>
       <c r="BD16" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE16" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF16" s="1">
-        <v>3</v>
+        <v>520</v>
+      </c>
+      <c r="BE16" s="3"/>
+      <c r="BF16" s="3">
+        <v>44645.936782407</v>
       </c>
       <c r="BG16" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH16" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI16" s="4">
-        <v>0.99</v>
+        <v>0</v>
+      </c>
+      <c r="BI16" s="1">
+        <v>2</v>
       </c>
       <c r="BJ16" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="BK16" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL16" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM16" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="BN16" s="1">
+        <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>120</v>
       </c>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F17" s="3">
         <v>44526.409328704001</v>
@@ -3703,55 +3884,55 @@
         <v>5</v>
       </c>
       <c r="AL17" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AM17" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AN17" s="2" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="AO17" s="1">
         <v>205</v>
       </c>
       <c r="AP17" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AQ17" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR17" s="2"/>
-      <c r="AS17" s="1"/>
+        <v>91</v>
+      </c>
+      <c r="AQ17" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR17" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS17" s="2"/>
       <c r="AT17" s="1"/>
       <c r="AU17" s="1"/>
-      <c r="AV17" s="2"/>
-      <c r="AW17" s="1">
-        <v>3594</v>
-      </c>
+      <c r="AV17" s="1"/>
+      <c r="AW17" s="2"/>
       <c r="AX17" s="1">
-        <v>22</v>
-      </c>
-      <c r="AY17" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY17" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AZ17" s="1">
+        <v>2</v>
+      </c>
+      <c r="BA17" s="1">
+        <v>3615</v>
+      </c>
+      <c r="BB17" s="1">
+        <v>59</v>
+      </c>
+      <c r="BC17" s="1">
         <v>273</v>
       </c>
-      <c r="AZ17" s="1">
-        <v>359</v>
-      </c>
-      <c r="BA17" s="3"/>
-      <c r="BB17" s="3">
-        <v>44526.454340277996</v>
-      </c>
-      <c r="BC17" s="1">
-        <v>1</v>
-      </c>
       <c r="BD17" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE17" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF17" s="1">
-        <v>3</v>
+        <v>428</v>
+      </c>
+      <c r="BE17" s="3"/>
+      <c r="BF17" s="3">
+        <v>44645.938483796002</v>
       </c>
       <c r="BG17" s="1">
         <v>0</v>
@@ -3759,24 +3940,36 @@
       <c r="BH17" s="1">
         <v>0</v>
       </c>
-      <c r="BI17" s="4">
-        <v>1.22</v>
+      <c r="BI17" s="1">
+        <v>2</v>
       </c>
       <c r="BJ17" s="1">
-        <v>51</v>
+        <v>3</v>
+      </c>
+      <c r="BK17" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL17" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM17" s="4">
+        <v>0.81</v>
+      </c>
+      <c r="BN17" s="1">
+        <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>121</v>
       </c>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F18" s="3">
         <v>44547.437592593</v>
@@ -3875,65 +4068,61 @@
         <v>0</v>
       </c>
       <c r="AL18" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM18" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AN18" s="2" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="AO18" s="1">
         <v>112</v>
       </c>
       <c r="AP18" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AQ18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR18" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AS18" s="1">
-        <v>10</v>
+        <v>92</v>
+      </c>
+      <c r="AQ18" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AR18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS18" s="2" t="s">
+        <v>83</v>
       </c>
       <c r="AT18" s="1">
         <v>10</v>
       </c>
       <c r="AU18" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV18" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW18" s="1">
-        <v>1604</v>
-      </c>
-      <c r="AX18" s="1">
-        <v>57</v>
-      </c>
-      <c r="AY18" s="1">
+        <v>10</v>
+      </c>
+      <c r="AV18" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW18" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX18" s="1"/>
+      <c r="AY18" s="2"/>
+      <c r="AZ18" s="1">
+        <v>1</v>
+      </c>
+      <c r="BA18" s="1">
+        <v>1619</v>
+      </c>
+      <c r="BB18" s="1">
+        <v>66</v>
+      </c>
+      <c r="BC18" s="1">
         <v>153</v>
       </c>
-      <c r="AZ18" s="1">
-        <v>1814</v>
-      </c>
-      <c r="BA18" s="3"/>
-      <c r="BB18" s="3">
-        <v>44547.458587963003</v>
-      </c>
-      <c r="BC18" s="1">
-        <v>1</v>
-      </c>
       <c r="BD18" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE18" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF18" s="1">
-        <v>3</v>
+        <v>1838</v>
+      </c>
+      <c r="BE18" s="3"/>
+      <c r="BF18" s="3">
+        <v>44645.939259259001</v>
       </c>
       <c r="BG18" s="1">
         <v>0</v>
@@ -3941,24 +4130,36 @@
       <c r="BH18" s="1">
         <v>0</v>
       </c>
-      <c r="BI18" s="4">
-        <v>0.91</v>
+      <c r="BI18" s="1">
+        <v>2</v>
       </c>
       <c r="BJ18" s="1">
+        <v>3</v>
+      </c>
+      <c r="BK18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL18" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM18" s="4">
+        <v>0.93</v>
+      </c>
+      <c r="BN18" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>122</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F19" s="3">
         <v>44568.452210648</v>
@@ -4057,80 +4258,92 @@
         <v>12</v>
       </c>
       <c r="AL19" s="2" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="AM19" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AN19" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AO19" s="1">
         <v>206</v>
       </c>
       <c r="AP19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AQ19" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR19" s="2"/>
-      <c r="AS19" s="1"/>
+        <v>96</v>
+      </c>
+      <c r="AQ19" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR19" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS19" s="2"/>
       <c r="AT19" s="1"/>
       <c r="AU19" s="1"/>
-      <c r="AV19" s="2"/>
-      <c r="AW19" s="1">
-        <v>63</v>
-      </c>
+      <c r="AV19" s="1"/>
+      <c r="AW19" s="2"/>
       <c r="AX19" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY19" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AZ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA19" s="1">
+        <v>82</v>
+      </c>
+      <c r="BB19" s="1">
+        <v>71</v>
+      </c>
+      <c r="BC19" s="1">
+        <v>159</v>
+      </c>
+      <c r="BD19" s="1">
+        <v>312</v>
+      </c>
+      <c r="BE19" s="3"/>
+      <c r="BF19" s="3">
+        <v>44645.940358795997</v>
+      </c>
+      <c r="BG19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI19" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ19" s="1">
+        <v>3</v>
+      </c>
+      <c r="BK19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL19" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM19" s="4">
+        <v>1.25</v>
+      </c>
+      <c r="BN19" s="1">
         <v>13</v>
       </c>
-      <c r="AY19" s="1">
-        <v>159</v>
-      </c>
-      <c r="AZ19" s="1">
-        <v>235</v>
-      </c>
-      <c r="BA19" s="3"/>
-      <c r="BB19" s="3">
-        <v>44568.454930555999</v>
-      </c>
-      <c r="BC19" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD19" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE19" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF19" s="1">
-        <v>3</v>
-      </c>
-      <c r="BG19" s="1">
-        <v>0</v>
-      </c>
-      <c r="BH19" s="1">
-        <v>0</v>
-      </c>
-      <c r="BI19" s="4">
-        <v>1.7</v>
-      </c>
-      <c r="BJ19" s="1">
-        <v>99</v>
-      </c>
     </row>
-    <row r="20" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>123</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F20" s="3">
         <v>44571.542523147997</v>
@@ -4229,88 +4442,96 @@
         <v>0</v>
       </c>
       <c r="AL20" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM20" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="AN20" s="2"/>
       <c r="AO20" s="1">
         <v>113</v>
       </c>
       <c r="AP20" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR20" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AQ20" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS20" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT20" s="1">
+        <v>50</v>
+      </c>
+      <c r="AU20" s="1">
+        <v>12</v>
+      </c>
+      <c r="AV20" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX20" s="1"/>
+      <c r="AY20" s="2"/>
+      <c r="AZ20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA20" s="1">
+        <v>2504</v>
+      </c>
+      <c r="BB20" s="1">
         <v>87</v>
       </c>
-      <c r="AS20" s="1">
-        <v>50</v>
-      </c>
-      <c r="AT20" s="1">
-        <v>12</v>
-      </c>
-      <c r="AU20" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV20" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW20" s="1">
-        <v>2488</v>
-      </c>
-      <c r="AX20" s="1">
-        <v>75</v>
-      </c>
-      <c r="AY20" s="1">
+      <c r="BC20" s="1">
         <v>99</v>
       </c>
-      <c r="AZ20" s="1">
-        <v>238</v>
-      </c>
-      <c r="BA20" s="3"/>
-      <c r="BB20" s="3">
-        <v>44571.573344907003</v>
-      </c>
-      <c r="BC20" s="1">
-        <v>1</v>
-      </c>
       <c r="BD20" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE20" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF20" s="1">
-        <v>3</v>
+        <v>282</v>
+      </c>
+      <c r="BE20" s="3"/>
+      <c r="BF20" s="3">
+        <v>44645.940902777998</v>
       </c>
       <c r="BG20" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH20" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI20" s="4">
-        <v>0.99</v>
+        <v>0</v>
+      </c>
+      <c r="BI20" s="1">
+        <v>2</v>
       </c>
       <c r="BJ20" s="1">
-        <v>16</v>
+        <v>3</v>
+      </c>
+      <c r="BK20" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL20" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM20" s="4">
+        <v>1.01</v>
+      </c>
+      <c r="BN20" s="1">
+        <v>17</v>
       </c>
     </row>
-    <row r="21" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>143</v>
       </c>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E21" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F21" s="3">
         <v>44572.677210647998</v>
@@ -4409,88 +4630,96 @@
         <v>0</v>
       </c>
       <c r="AL21" s="2" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="AM21" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AN21" s="2"/>
       <c r="AO21" s="1">
         <v>114</v>
       </c>
       <c r="AP21" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="AQ21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR21" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS21" s="1">
+        <v>110</v>
+      </c>
+      <c r="AQ21" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="AR21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS21" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT21" s="1">
         <v>40</v>
       </c>
-      <c r="AT21" s="1">
+      <c r="AU21" s="1">
         <v>28</v>
       </c>
-      <c r="AU21" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV21" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AW21" s="1">
-        <v>64</v>
-      </c>
-      <c r="AX21" s="1">
-        <v>176</v>
-      </c>
-      <c r="AY21" s="1">
+      <c r="AV21" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW21" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AX21" s="1"/>
+      <c r="AY21" s="2"/>
+      <c r="AZ21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA21" s="1">
+        <v>84</v>
+      </c>
+      <c r="BB21" s="1">
+        <v>182</v>
+      </c>
+      <c r="BC21" s="1">
         <v>210</v>
       </c>
-      <c r="AZ21" s="1">
-        <v>450</v>
-      </c>
-      <c r="BA21" s="3"/>
-      <c r="BB21" s="3">
-        <v>44572.682418981</v>
-      </c>
-      <c r="BC21" s="1">
-        <v>1</v>
-      </c>
       <c r="BD21" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE21" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF21" s="1">
-        <v>3</v>
+        <v>476</v>
+      </c>
+      <c r="BE21" s="3"/>
+      <c r="BF21" s="3">
+        <v>44645.941354167</v>
       </c>
       <c r="BG21" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH21" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI21" s="4">
-        <v>0.78</v>
+        <v>0</v>
+      </c>
+      <c r="BI21" s="1">
+        <v>2</v>
       </c>
       <c r="BJ21" s="1">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="BK21" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL21" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM21" s="4">
+        <v>0.85</v>
+      </c>
+      <c r="BN21" s="1">
+        <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>144</v>
       </c>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F22" s="3">
         <v>44578.401655093003</v>
@@ -4589,78 +4818,90 @@
         <v>9</v>
       </c>
       <c r="AL22" s="2" t="s">
-        <v>101</v>
+        <v>112</v>
       </c>
       <c r="AM22" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AN22" s="2"/>
       <c r="AO22" s="1">
         <v>207</v>
       </c>
       <c r="AP22" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AQ22" s="1">
-        <v>2</v>
-      </c>
-      <c r="AR22" s="2"/>
-      <c r="AS22" s="1"/>
+        <v>112</v>
+      </c>
+      <c r="AQ22" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR22" s="1">
+        <v>2</v>
+      </c>
+      <c r="AS22" s="2"/>
       <c r="AT22" s="1"/>
       <c r="AU22" s="1"/>
-      <c r="AV22" s="2"/>
-      <c r="AW22" s="1">
-        <v>3868</v>
-      </c>
+      <c r="AV22" s="1"/>
+      <c r="AW22" s="2"/>
       <c r="AX22" s="1">
+        <v>1</v>
+      </c>
+      <c r="AY22" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AZ22" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA22" s="1">
+        <v>3884</v>
+      </c>
+      <c r="BB22" s="1">
+        <v>52</v>
+      </c>
+      <c r="BC22" s="1">
+        <v>187</v>
+      </c>
+      <c r="BD22" s="1">
+        <v>335</v>
+      </c>
+      <c r="BE22" s="3"/>
+      <c r="BF22" s="3">
+        <v>44645.942349536999</v>
+      </c>
+      <c r="BG22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BH22" s="1">
+        <v>0</v>
+      </c>
+      <c r="BI22" s="1">
+        <v>2</v>
+      </c>
+      <c r="BJ22" s="1">
+        <v>3</v>
+      </c>
+      <c r="BK22" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL22" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM22" s="4">
+        <v>0.99</v>
+      </c>
+      <c r="BN22" s="1">
         <v>17</v>
       </c>
-      <c r="AY22" s="1">
-        <v>187</v>
-      </c>
-      <c r="AZ22" s="1">
-        <v>268</v>
-      </c>
-      <c r="BA22" s="3"/>
-      <c r="BB22" s="3">
-        <v>44578.448784722001</v>
-      </c>
-      <c r="BC22" s="1">
-        <v>1</v>
-      </c>
-      <c r="BD22" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE22" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF22" s="1">
-        <v>3</v>
-      </c>
-      <c r="BG22" s="1">
-        <v>3</v>
-      </c>
-      <c r="BH22" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI22" s="4">
-        <v>1.32</v>
-      </c>
-      <c r="BJ22" s="1">
-        <v>71</v>
-      </c>
     </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>145</v>
       </c>
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F23" s="3">
         <v>44580.388784722003</v>
@@ -4759,63 +5000,59 @@
         <v>0</v>
       </c>
       <c r="AL23" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM23" s="2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="AN23" s="2" t="s">
-        <v>103</v>
+        <v>115</v>
       </c>
       <c r="AO23" s="1">
         <v>115</v>
       </c>
       <c r="AP23" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ23" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR23" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="AS23" s="1">
+        <v>78</v>
+      </c>
+      <c r="AQ23" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="AR23" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS23" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AT23" s="1">
         <v>45</v>
       </c>
-      <c r="AT23" s="1">
+      <c r="AU23" s="1">
         <v>16</v>
       </c>
-      <c r="AU23" s="1">
-        <v>2</v>
-      </c>
-      <c r="AV23" s="2"/>
-      <c r="AW23" s="1">
-        <v>3715</v>
-      </c>
-      <c r="AX23" s="1">
-        <v>168</v>
-      </c>
-      <c r="AY23" s="1">
+      <c r="AV23" s="1">
+        <v>2</v>
+      </c>
+      <c r="AW23" s="2"/>
+      <c r="AX23" s="1"/>
+      <c r="AY23" s="2"/>
+      <c r="AZ23" s="1">
+        <v>4</v>
+      </c>
+      <c r="BA23" s="1">
+        <v>3740</v>
+      </c>
+      <c r="BB23" s="1">
+        <v>184</v>
+      </c>
+      <c r="BC23" s="1">
         <v>120</v>
       </c>
-      <c r="AZ23" s="1">
-        <v>352</v>
-      </c>
-      <c r="BA23" s="3"/>
-      <c r="BB23" s="3">
-        <v>44580.435115740998</v>
-      </c>
-      <c r="BC23" s="1">
-        <v>1</v>
-      </c>
       <c r="BD23" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE23" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF23" s="1">
-        <v>3</v>
+        <v>400</v>
+      </c>
+      <c r="BE23" s="3"/>
+      <c r="BF23" s="3">
+        <v>44645.942974537</v>
       </c>
       <c r="BG23" s="1">
         <v>0</v>
@@ -4823,24 +5060,36 @@
       <c r="BH23" s="1">
         <v>0</v>
       </c>
-      <c r="BI23" s="4">
-        <v>0.67</v>
+      <c r="BI23" s="1">
+        <v>2</v>
       </c>
       <c r="BJ23" s="1">
+        <v>3</v>
+      </c>
+      <c r="BK23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL23" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM23" s="4">
+        <v>0.69</v>
+      </c>
+      <c r="BN23" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="24" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>146</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F24" s="3">
         <v>44585.549328704001</v>
@@ -4939,88 +5188,96 @@
         <v>0</v>
       </c>
       <c r="AL24" s="2" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="AM24" s="2" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
       <c r="AN24" s="2"/>
       <c r="AO24" s="1">
         <v>116</v>
       </c>
       <c r="AP24" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="AQ24" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR24" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="AS24" s="1">
-        <v>3</v>
+        <v>100</v>
+      </c>
+      <c r="AQ24" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS24" s="2" t="s">
+        <v>108</v>
       </c>
       <c r="AT24" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AU24" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV24" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="AW24" s="1">
-        <v>2602</v>
-      </c>
-      <c r="AX24" s="1">
-        <v>96</v>
-      </c>
-      <c r="AY24" s="1">
+        <v>4</v>
+      </c>
+      <c r="AV24" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW24" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AX24" s="1"/>
+      <c r="AY24" s="2"/>
+      <c r="AZ24" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA24" s="1">
+        <v>2616</v>
+      </c>
+      <c r="BB24" s="1">
+        <v>104</v>
+      </c>
+      <c r="BC24" s="1">
         <v>170</v>
       </c>
-      <c r="AZ24" s="1">
-        <v>330</v>
-      </c>
-      <c r="BA24" s="3"/>
-      <c r="BB24" s="3">
-        <v>44585.582534722002</v>
-      </c>
-      <c r="BC24" s="1">
-        <v>1</v>
-      </c>
       <c r="BD24" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE24" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF24" s="1">
-        <v>3</v>
+        <v>370</v>
+      </c>
+      <c r="BE24" s="3"/>
+      <c r="BF24" s="3">
+        <v>44645.943414351997</v>
       </c>
       <c r="BG24" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH24" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI24" s="4">
-        <v>0.66</v>
+        <v>0</v>
+      </c>
+      <c r="BI24" s="1">
+        <v>2</v>
       </c>
       <c r="BJ24" s="1">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="BK24" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL24" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM24" s="4">
+        <v>0.7</v>
+      </c>
+      <c r="BN24" s="1">
+        <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>147</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E25" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F25" s="3">
         <v>44592.570231480997</v>
@@ -5119,65 +5376,61 @@
         <v>0</v>
       </c>
       <c r="AL25" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AM25" s="2" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="AN25" s="2" t="s">
-        <v>107</v>
+        <v>118</v>
       </c>
       <c r="AO25" s="1">
         <v>117</v>
       </c>
       <c r="AP25" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="AQ25" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="AQ25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR25" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="AS25" s="1">
+      <c r="AT25" s="1">
         <v>5</v>
       </c>
-      <c r="AT25" s="1">
-        <v>0</v>
-      </c>
       <c r="AU25" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV25" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="AW25" s="1">
-        <v>56</v>
-      </c>
-      <c r="AX25" s="1">
-        <v>158</v>
-      </c>
-      <c r="AY25" s="1">
+        <v>0</v>
+      </c>
+      <c r="AV25" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW25" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AX25" s="1"/>
+      <c r="AY25" s="2"/>
+      <c r="AZ25" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA25" s="1">
+        <v>198</v>
+      </c>
+      <c r="BB25" s="1">
+        <v>171</v>
+      </c>
+      <c r="BC25" s="1">
         <v>220</v>
       </c>
-      <c r="AZ25" s="1">
-        <v>434</v>
-      </c>
-      <c r="BA25" s="3"/>
-      <c r="BB25" s="3">
-        <v>44592.575254629999</v>
-      </c>
-      <c r="BC25" s="1">
-        <v>1</v>
-      </c>
       <c r="BD25" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE25" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF25" s="1">
-        <v>3</v>
+        <v>589</v>
+      </c>
+      <c r="BE25" s="3"/>
+      <c r="BF25" s="3">
+        <v>44645.945416666997</v>
       </c>
       <c r="BG25" s="1">
         <v>0</v>
@@ -5185,24 +5438,36 @@
       <c r="BH25" s="1">
         <v>0</v>
       </c>
-      <c r="BI25" s="4">
-        <v>0.83</v>
+      <c r="BI25" s="1">
+        <v>2</v>
       </c>
       <c r="BJ25" s="1">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="BK25" s="1">
+        <v>0</v>
+      </c>
+      <c r="BL25" s="1">
+        <v>0</v>
+      </c>
+      <c r="BM25" s="4">
+        <v>0.63</v>
+      </c>
+      <c r="BN25" s="1">
+        <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>148</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F26" s="3">
         <v>44606.494259259001</v>
@@ -5301,88 +5566,96 @@
         <v>0</v>
       </c>
       <c r="AL26" s="2" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="AM26" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AN26" s="2"/>
       <c r="AO26" s="1">
         <v>118</v>
       </c>
       <c r="AP26" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="AQ26" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="AR26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS26" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="AQ26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR26" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="AS26" s="1">
+      <c r="AT26" s="1">
         <v>10</v>
       </c>
-      <c r="AT26" s="1">
+      <c r="AU26" s="1">
         <v>6</v>
       </c>
-      <c r="AU26" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV26" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW26" s="1">
-        <v>54</v>
-      </c>
-      <c r="AX26" s="1">
-        <v>58</v>
-      </c>
-      <c r="AY26" s="1">
+      <c r="AV26" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW26" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX26" s="1"/>
+      <c r="AY26" s="2"/>
+      <c r="AZ26" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA26" s="1">
+        <v>73</v>
+      </c>
+      <c r="BB26" s="1">
+        <v>65</v>
+      </c>
+      <c r="BC26" s="1">
         <v>166</v>
       </c>
-      <c r="AZ26" s="1">
-        <v>278</v>
-      </c>
-      <c r="BA26" s="3"/>
-      <c r="BB26" s="3">
-        <v>44606.497476851997</v>
-      </c>
-      <c r="BC26" s="1">
-        <v>1</v>
-      </c>
       <c r="BD26" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE26" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF26" s="1">
-        <v>3</v>
+        <v>304</v>
+      </c>
+      <c r="BE26" s="3"/>
+      <c r="BF26" s="3">
+        <v>44645.945914352</v>
       </c>
       <c r="BG26" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH26" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI26" s="4">
-        <v>1.25</v>
+        <v>0</v>
+      </c>
+      <c r="BI26" s="1">
+        <v>2</v>
       </c>
       <c r="BJ26" s="1">
-        <v>13</v>
+        <v>3</v>
+      </c>
+      <c r="BK26" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL26" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM26" s="4">
+        <v>1.33</v>
+      </c>
+      <c r="BN26" s="1">
+        <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>149</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F27" s="3">
         <v>44608.485983796003</v>
@@ -5481,86 +5754,94 @@
         <v>0</v>
       </c>
       <c r="AL27" s="2" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
       <c r="AM27" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="AN27" s="2"/>
       <c r="AO27" s="1">
         <v>119</v>
       </c>
       <c r="AP27" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AQ27" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR27" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="AS27" s="1">
+        <v>73</v>
+      </c>
+      <c r="AQ27" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AR27" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS27" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AT27" s="1">
         <v>26</v>
       </c>
-      <c r="AT27" s="1">
+      <c r="AU27" s="1">
         <v>8</v>
       </c>
-      <c r="AU27" s="1">
-        <v>2</v>
-      </c>
-      <c r="AV27" s="2"/>
-      <c r="AW27" s="1">
-        <v>82</v>
-      </c>
-      <c r="AX27" s="1">
-        <v>103</v>
-      </c>
-      <c r="AY27" s="1">
+      <c r="AV27" s="1">
+        <v>2</v>
+      </c>
+      <c r="AW27" s="2"/>
+      <c r="AX27" s="1"/>
+      <c r="AY27" s="2"/>
+      <c r="AZ27" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA27" s="1">
+        <v>96</v>
+      </c>
+      <c r="BB27" s="1">
+        <v>116</v>
+      </c>
+      <c r="BC27" s="1">
         <v>151</v>
       </c>
-      <c r="AZ27" s="1">
-        <v>336</v>
-      </c>
-      <c r="BA27" s="3"/>
-      <c r="BB27" s="3">
-        <v>44608.489884258997</v>
-      </c>
-      <c r="BC27" s="1">
-        <v>1</v>
-      </c>
       <c r="BD27" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE27" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF27" s="1">
-        <v>3</v>
+        <v>363</v>
+      </c>
+      <c r="BE27" s="3"/>
+      <c r="BF27" s="3">
+        <v>44645.946666666998</v>
       </c>
       <c r="BG27" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH27" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI27" s="4">
-        <v>0.93</v>
+        <v>0</v>
+      </c>
+      <c r="BI27" s="1">
+        <v>2</v>
       </c>
       <c r="BJ27" s="1">
         <v>3</v>
       </c>
+      <c r="BK27" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL27" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM27" s="4">
+        <v>1.03</v>
+      </c>
+      <c r="BN27" s="1">
+        <v>3</v>
+      </c>
     </row>
-    <row r="28" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>150</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F28" s="3">
         <v>44620.585578703998</v>
@@ -5659,88 +5940,96 @@
         <v>0</v>
       </c>
       <c r="AL28" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM28" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AN28" s="2"/>
       <c r="AO28" s="1">
         <v>120</v>
       </c>
       <c r="AP28" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="AQ28" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR28" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AS28" s="1">
+        <v>78</v>
+      </c>
+      <c r="AQ28" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS28" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="AT28" s="1">
         <v>40</v>
       </c>
-      <c r="AT28" s="1">
+      <c r="AU28" s="1">
         <v>12</v>
       </c>
-      <c r="AU28" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV28" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="AW28" s="1">
-        <v>3310</v>
-      </c>
-      <c r="AX28" s="1">
-        <v>111</v>
-      </c>
-      <c r="AY28" s="1">
+      <c r="AV28" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW28" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AX28" s="1"/>
+      <c r="AY28" s="2"/>
+      <c r="AZ28" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA28" s="1">
+        <v>3329</v>
+      </c>
+      <c r="BB28" s="1">
+        <v>117</v>
+      </c>
+      <c r="BC28" s="1">
         <v>162</v>
       </c>
-      <c r="AZ28" s="1">
-        <v>337</v>
-      </c>
-      <c r="BA28" s="3"/>
-      <c r="BB28" s="3">
-        <v>44620.627048611001</v>
-      </c>
-      <c r="BC28" s="1">
-        <v>1</v>
-      </c>
       <c r="BD28" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE28" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF28" s="1">
-        <v>3</v>
+        <v>375</v>
+      </c>
+      <c r="BE28" s="3"/>
+      <c r="BF28" s="3">
+        <v>44645.947094907002</v>
       </c>
       <c r="BG28" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH28" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI28" s="4">
-        <v>0.63</v>
+        <v>0</v>
+      </c>
+      <c r="BI28" s="1">
+        <v>2</v>
       </c>
       <c r="BJ28" s="1">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="BK28" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL28" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM28" s="4">
+        <v>0.67</v>
+      </c>
+      <c r="BN28" s="1">
+        <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:62" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>151</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="F29" s="3">
         <v>44622.452106481003</v>
@@ -5839,75 +6128,83 @@
         <v>0</v>
       </c>
       <c r="AL29" s="2" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="AM29" s="2" t="s">
-        <v>75</v>
+        <v>82</v>
       </c>
       <c r="AN29" s="2"/>
       <c r="AO29" s="1">
         <v>121</v>
       </c>
       <c r="AP29" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ29" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="AR29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AS29" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="AQ29" s="1">
-        <v>1</v>
-      </c>
-      <c r="AR29" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="AS29" s="1">
+      <c r="AT29" s="1">
         <v>70</v>
       </c>
-      <c r="AT29" s="1">
+      <c r="AU29" s="1">
         <v>16</v>
       </c>
-      <c r="AU29" s="1">
-        <v>1</v>
-      </c>
-      <c r="AV29" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AW29" s="1">
-        <v>56</v>
-      </c>
-      <c r="AX29" s="1">
-        <v>222</v>
-      </c>
-      <c r="AY29" s="1">
+      <c r="AV29" s="1">
+        <v>1</v>
+      </c>
+      <c r="AW29" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AX29" s="1"/>
+      <c r="AY29" s="2"/>
+      <c r="AZ29" s="1">
+        <v>3</v>
+      </c>
+      <c r="BA29" s="1">
+        <v>72</v>
+      </c>
+      <c r="BB29" s="1">
+        <v>248</v>
+      </c>
+      <c r="BC29" s="1">
         <v>205</v>
       </c>
-      <c r="AZ29" s="1">
-        <v>483</v>
-      </c>
-      <c r="BA29" s="3"/>
-      <c r="BB29" s="3">
-        <v>44622.457708333</v>
-      </c>
-      <c r="BC29" s="1">
-        <v>1</v>
-      </c>
       <c r="BD29" s="1">
-        <v>0</v>
-      </c>
-      <c r="BE29" s="1">
-        <v>3</v>
-      </c>
-      <c r="BF29" s="1">
-        <v>3</v>
+        <v>525</v>
+      </c>
+      <c r="BE29" s="3"/>
+      <c r="BF29" s="3">
+        <v>44645.948090277998</v>
       </c>
       <c r="BG29" s="1">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BH29" s="1">
-        <v>1</v>
-      </c>
-      <c r="BI29" s="4">
-        <v>0.8</v>
+        <v>0</v>
+      </c>
+      <c r="BI29" s="1">
+        <v>2</v>
       </c>
       <c r="BJ29" s="1">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="BK29" s="1">
+        <v>3</v>
+      </c>
+      <c r="BL29" s="1">
+        <v>1</v>
+      </c>
+      <c r="BM29" s="4">
+        <v>0.87</v>
+      </c>
+      <c r="BN29" s="1">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>